<commit_message>
Added Digi-Key Stock Information
</commit_message>
<xml_diff>
--- a/DataManagementBoard_V3.31/Bill of Materials-DataManagementBoard_V3.xlsx
+++ b/DataManagementBoard_V3.31/Bill of Materials-DataManagementBoard_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2020 - 2021\Andromeda-V3.2\DataManagementBoard_V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noorg\OneDrive\Documents\GitHub\Andromeda-V3.3\DataManagementBoard_V3.31\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A06DC4A-E943-491A-9C4A-69C22D781BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251DC166-7FB5-47C3-9ABC-67B86E2F19B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15690" yWindow="2670" windowWidth="14400" windowHeight="7365" xr2:uid="{3D4BD06D-1139-467C-B010-4B4921899CC2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{3D4BD06D-1139-467C-B010-4B4921899CC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-DataManagemen" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
   <si>
     <t>Comment</t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>C7, C19</t>
+  </si>
+  <si>
+    <t>Availability as of 04-04-22</t>
+  </si>
+  <si>
+    <t>In Stock</t>
+  </si>
+  <si>
+    <t>Normally Stocking</t>
+  </si>
+  <si>
+    <t>Non-Stock</t>
   </si>
 </sst>
 </file>
@@ -348,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,12 +372,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -677,18 +706,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -707,8 +737,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G1" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -727,8 +760,11 @@
       <c r="F2" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="G2" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -747,8 +783,11 @@
       <c r="F3" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G3" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -767,8 +806,11 @@
       <c r="F4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G4" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -787,8 +829,11 @@
       <c r="F5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G5" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -807,8 +852,11 @@
       <c r="F6" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G6" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -827,8 +875,11 @@
       <c r="F7" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G7" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -847,8 +898,11 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G8" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -867,8 +921,11 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G9" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -887,8 +944,11 @@
       <c r="F10" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G10" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -907,8 +967,11 @@
       <c r="F11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G11" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -927,8 +990,11 @@
       <c r="F12" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G12" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -947,8 +1013,11 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G13" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -967,8 +1036,11 @@
       <c r="F14" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G14" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -987,8 +1059,11 @@
       <c r="F15" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G15" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -1007,8 +1082,11 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G16" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -1027,8 +1105,11 @@
       <c r="F17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G17" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
@@ -1047,8 +1128,11 @@
       <c r="F18" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G18" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1067,8 +1151,11 @@
       <c r="F19" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G19" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
@@ -1087,8 +1174,11 @@
       <c r="F20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G20" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>64</v>
       </c>
@@ -1107,8 +1197,11 @@
       <c r="F21" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G21" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>68</v>
       </c>
@@ -1127,8 +1220,11 @@
       <c r="F22" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G22" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
@@ -1147,8 +1243,11 @@
       <c r="F23" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G23" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
@@ -1167,8 +1266,11 @@
       <c r="F24" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G24" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>77</v>
       </c>
@@ -1187,8 +1289,11 @@
       <c r="F25" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G25" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>81</v>
       </c>
@@ -1207,8 +1312,16 @@
       <c r="F26" s="4">
         <v>1</v>
       </c>
+      <c r="G26" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:G26">
+    <cfRule type="notContainsText" dxfId="0" priority="1" operator="notContains" text="In Stock">
+      <formula>ISERROR(SEARCH("In Stock",G2))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" blackAndWhite="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>